<commit_message>
Updated Version. Fixed all typos. Released to public.
</commit_message>
<xml_diff>
--- a/_templates/Operational-Logistics-Board/Jobs_Meta_Information_en.xlsx
+++ b/_templates/Operational-Logistics-Board/Jobs_Meta_Information_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Operational_Logistics_Board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Operational-Logistics-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31534808-A5AA-E74C-89FB-FCE9150FB5C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DF6572-C73A-7240-8E41-DF62700D64CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46520" yWindow="-4060" windowWidth="36780" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34400" yWindow="-3280" windowWidth="36780" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,6 @@
     <t>Hans Meier Ind.</t>
   </si>
   <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>High Priority</t>
-  </si>
-  <si>
     <t>Schmitt Retirement Home</t>
   </si>
   <si>
@@ -53,6 +47,12 @@
   </si>
   <si>
     <t>job_prio</t>
+  </si>
+  <si>
+    <t>Standard Order</t>
+  </si>
+  <si>
+    <t>Urgent Order</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D869"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -430,7 +430,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -447,10 +447,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -461,10 +461,10 @@
         <v>900</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -475,10 +475,10 @@
         <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -489,7 +489,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
@@ -503,10 +503,10 @@
         <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>